<commit_message>
Extensive updates and notes
Updates to motor control code, Brigand combat code, and many other areas as well as some cleanup.

Excel spreadsheet has been updated with more information.
</commit_message>
<xml_diff>
--- a/Dark Tower RAM usage.xlsx
+++ b/Dark Tower RAM usage.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work in progress\Dark Tower\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work in progress\github\Dark-Tower\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DDF70B-BAC5-4047-AA09-2F935F57F294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="2295"/>
+    <workbookView xWindow="-21705" yWindow="3420" windowWidth="21000" windowHeight="22050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>X = 0</t>
   </si>
@@ -123,10 +135,6 @@
   </si>
   <si>
     <t>0b0010 - Brass key</t>
-  </si>
-  <si>
-    <t>???
-Init 15</t>
   </si>
   <si>
     <t>Sound
@@ -343,10 +351,6 @@
   </si>
   <si>
     <t>Current
-Player</t>
-  </si>
-  <si>
-    <t>Current
 Barrel
 Position</t>
   </si>
@@ -461,9 +465,6 @@
     <t>Note 5:</t>
   </si>
   <si>
-    <t>0b0100 -</t>
-  </si>
-  <si>
     <t>Base 10 Addition
 and Subtraction</t>
   </si>
@@ -473,9 +474,6 @@
   </si>
   <si>
     <t>0b0001 - Key not found yet</t>
-  </si>
-  <si>
-    <t>0/3 appears to be player status flags</t>
   </si>
   <si>
     <t>0b0010 - Cursed when clear</t>
@@ -559,9 +557,6 @@
 Clear routine</t>
   </si>
   <si>
-    <t>Bazaar Pricing Information</t>
-  </si>
-  <si>
     <t>Current
 Bazaar
 Item</t>
@@ -580,18 +575,102 @@
 Attempted</t>
   </si>
   <si>
-    <t>LED
-Flags</t>
-  </si>
-  <si>
     <t>Prev Key
 Pressed?</t>
+  </si>
+  <si>
+    <t>HO Barrel
+Timer
+Init 15</t>
+  </si>
+  <si>
+    <t>LO Barrel
+Timer
+Init 15</t>
+  </si>
+  <si>
+    <t>Note 6:</t>
+  </si>
+  <si>
+    <t>Flags
+Note 6</t>
+  </si>
+  <si>
+    <t>0b0100 - Immediate LED update (no blinking)</t>
+  </si>
+  <si>
+    <t>0b1000 - Which digit of the LED display is actively being refreshed - 1=10s digit; 0=1s digit</t>
+  </si>
+  <si>
+    <t>0b0010 - LED blinking status - 0=data is displayed; 1=display is blank</t>
+  </si>
+  <si>
+    <t>Flags
+Note 7</t>
+  </si>
+  <si>
+    <t>Note 7:</t>
+  </si>
+  <si>
+    <t>6/13 contains various unrelated flags</t>
+  </si>
+  <si>
+    <t>0b0001 - BCD or Raw display - 0=BCD; 1=Raw</t>
+  </si>
+  <si>
+    <t>0b0010 - Prompt - 0=Game running; 1=Waiting for user input</t>
+  </si>
+  <si>
+    <t>0b1000 - Keypress detected (play tick sound) - 0=waiting for input; 1=keypress detected</t>
+  </si>
+  <si>
+    <t>0b0001 - Wait for input - 1=Wait for a keypress, 0=Do not wait for a keypress (just check once)</t>
+  </si>
+  <si>
+    <t>6/12 contains various flags, most related to the LED display</t>
+  </si>
+  <si>
+    <t>0b0100 - Unused.  Was potentially a mute function</t>
+  </si>
+  <si>
+    <t>0b1000 - Not used</t>
+  </si>
+  <si>
+    <t>0b0100 - Not used</t>
+  </si>
+  <si>
+    <t>Bazaar Warrior Price</t>
+  </si>
+  <si>
+    <t>Bazaar Beast Price</t>
+  </si>
+  <si>
+    <t>Bazaar Scout Price</t>
+  </si>
+  <si>
+    <t>Bazaar Healer Price</t>
+  </si>
+  <si>
+    <t>Bazaar Price Rotation Buffer</t>
+  </si>
+  <si>
+    <t>Current
+Player
+(0-3)</t>
+  </si>
+  <si>
+    <t>Temporary
+Current
+Player</t>
+  </si>
+  <si>
+    <t>0/3 Contains the player status flags</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -764,15 +843,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1008,312 +1078,322 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1594,55 +1674,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="1" customWidth="1"/>
     <col min="16" max="17" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1692,529 +1772,599 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="H3" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="K3" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="N3" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="52"/>
-    </row>
-    <row r="4" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="76"/>
+    </row>
+    <row r="4" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="E4" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="H4" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="K4" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="K4" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="N4" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="N4" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="O4" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="54"/>
-    </row>
-    <row r="5" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O4" s="77" t="s">
+        <v>119</v>
+      </c>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="79"/>
+    </row>
+    <row r="5" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="57" t="s">
+      <c r="B5" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="E5" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="86" t="s">
+      <c r="H5" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="K5" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="47" t="s">
+      <c r="N5" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="N5" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="O5" s="55"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="56"/>
-    </row>
-    <row r="6" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="81"/>
+    </row>
+    <row r="6" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="75" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="76"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="78" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="85"/>
-      <c r="G6" s="88" t="s">
-        <v>120</v>
-      </c>
-      <c r="H6" s="89"/>
-      <c r="I6" s="88" t="s">
-        <v>121</v>
-      </c>
-      <c r="J6" s="89"/>
-      <c r="K6" s="80" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="79" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="93" t="s">
-        <v>77</v>
-      </c>
-      <c r="N6" s="81" t="s">
+      <c r="B6" s="97" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="95"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="83"/>
+      <c r="G6" s="86" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="87"/>
+      <c r="I6" s="86" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="87"/>
+      <c r="K6" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="68" t="s">
+        <v>148</v>
+      </c>
+      <c r="N6" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="82" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="83" t="s">
+      <c r="P6" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="84" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:17" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="65" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="90" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="91" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="92"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="68" t="s">
+        <v>149</v>
+      </c>
+      <c r="N7" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q7" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="P7" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q7" s="22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="99" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="74" t="s">
-        <v>102</v>
-      </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="91" t="s">
-        <v>126</v>
-      </c>
-      <c r="N8" s="91" t="s">
-        <v>122</v>
-      </c>
-      <c r="O8" s="93" t="s">
-        <v>128</v>
-      </c>
-      <c r="P8" s="23" t="s">
+      <c r="B8" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="93"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="Q8" s="24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="N8" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="O8" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q8" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="62"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="92"/>
-      <c r="N9" s="100" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="O9" s="100" t="s">
+        <v>132</v>
+      </c>
+      <c r="P9" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q9" s="47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="50"/>
+      <c r="C10" s="88" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="89"/>
+      <c r="E10" s="88" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="89"/>
+      <c r="G10" s="88" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" s="89"/>
+      <c r="I10" s="88" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="89"/>
+      <c r="K10" s="88" t="s">
+        <v>147</v>
+      </c>
+      <c r="L10" s="90"/>
+      <c r="M10" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="N10" s="84" t="s">
+        <v>122</v>
+      </c>
+      <c r="O10" s="85"/>
+      <c r="P10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="98" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="98" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="15"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="15"/>
+      <c r="B33" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="15"/>
+      <c r="B34" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="15"/>
+      <c r="B35" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="15"/>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="15"/>
+      <c r="B38" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="15"/>
+      <c r="B39" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="15"/>
+      <c r="B40" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="15"/>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="98" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="15"/>
+      <c r="B43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="15"/>
+      <c r="B44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="15"/>
+      <c r="B45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="15"/>
+      <c r="B46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="15"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="98" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="99" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="99" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="O9" s="90" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="101" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q9" s="59" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="94" t="s">
-        <v>124</v>
-      </c>
-      <c r="D10" s="95"/>
-      <c r="E10" s="94" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="95"/>
-      <c r="G10" s="94" t="s">
-        <v>124</v>
-      </c>
-      <c r="H10" s="95"/>
-      <c r="I10" s="94" t="s">
-        <v>124</v>
-      </c>
-      <c r="J10" s="95"/>
-      <c r="K10" s="94" t="s">
-        <v>124</v>
-      </c>
-      <c r="L10" s="96"/>
-      <c r="M10" s="93" t="s">
-        <v>125</v>
-      </c>
-      <c r="N10" s="97" t="s">
-        <v>127</v>
-      </c>
-      <c r="O10" s="98"/>
-      <c r="P10" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="6"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="61" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="61" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="61" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="61" t="s">
-        <v>116</v>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="99" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="99" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2227,15 +2377,15 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="K10:L10"/>
+    <mergeCell ref="C7:D8"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="O3:Q3"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>